<commit_message>
Add TRA emission scenario (incomplete)
</commit_message>
<xml_diff>
--- a/SuppXLS/Scen_TRA_EMISSION.xlsx
+++ b/SuppXLS/Scen_TRA_EMISSION.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Irish-TIMES-model\SuppXLS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7ADA4224-463F-494F-81EA-9663608CA3B3}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D4E5470-E826-4AB8-97E9-50228772727A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1789,8 +1789,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:AR4"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="Y1" workbookViewId="0">
-      <selection activeCell="AQ5" sqref="AQ5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1815,7 +1815,7 @@
     <col min="44" max="44" width="8.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:44" ht="21.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>17</v>
       </c>

</xml_diff>